<commit_message>
Disable crude oil and heavy fuel oil plants in the US EPS
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D6EFB1-532C-499B-8BB2-D38B4746374B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE59DCF4-C3ED-4DFD-8048-6B73D6458F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
   <si>
     <t>Source:</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>hydrogen combined cycle</t>
+  </si>
+  <si>
+    <t>Heavy fuel oil and crude oil plants are not used in the US model.</t>
   </si>
 </sst>
 </file>
@@ -775,9 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -905,6 +910,11 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1353,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,8 +1501,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="14">
-        <f>B12</f>
-        <v>9000000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,8 +1509,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="14">
-        <f>B12</f>
-        <v>9000000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>